<commit_message>
prevent qr generation of batch having no accounts on database
</commit_message>
<xml_diff>
--- a/account_range.xlsx
+++ b/account_range.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gente\OneDrive\Desktop\node-qr-range\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E9593C-8FB1-4AD5-9670-B6E3FECFEB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8C9C89-A2DD-46EC-9D94-BCBDFF448031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>S.N</t>
   </si>
@@ -73,6 +73,21 @@
   </si>
   <si>
     <t>F-02-02</t>
+  </si>
+  <si>
+    <t>03200501200100</t>
+  </si>
+  <si>
+    <t>F-3</t>
+  </si>
+  <si>
+    <t>03200501200152</t>
+  </si>
+  <si>
+    <t>F-02-03</t>
+  </si>
+  <si>
+    <t>F- 33</t>
   </si>
 </sst>
 </file>
@@ -108,8 +123,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,7 +469,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -464,13 +480,36 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
-        <v>3200501200100</v>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3200501200101</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
         <v>12</v>
       </c>
     </row>

</xml_diff>